<commit_message>
Fixes of player movement.
</commit_message>
<xml_diff>
--- a/paths.xlsx
+++ b/paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PJATK\PPRG_exercises\PPRG_projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AC3177-57A1-4D48-A6F8-2A7F933439E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5EC06-9B22-4E7E-AC2A-9E0D3B0F905F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1095" yWindow="-120" windowWidth="27825" windowHeight="16440" activeTab="2" xr2:uid="{A46F3A4D-3F05-483C-ACB4-AA6AEC45270A}"/>
+    <workbookView xWindow="1095" yWindow="-120" windowWidth="27825" windowHeight="16440" activeTab="1" xr2:uid="{A46F3A4D-3F05-483C-ACB4-AA6AEC45270A}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz3" sheetId="5" r:id="rId1"/>
@@ -1730,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C609D67-88B5-450A-B191-704C0545D9B9}">
   <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,7 +2887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A683FC-490F-450E-B7F8-E05F0B95AC55}">
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>

</xml_diff>